<commit_message>
Modified Controller AppDependent AppIndependent UserModuleMethods files
</commit_message>
<xml_diff>
--- a/SG_Mvn_Project/ExecutionController/Controller.xlsx
+++ b/SG_Mvn_Project/ExecutionController/Controller.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>ProjectName</t>
   </si>
@@ -81,13 +81,17 @@
   </si>
   <si>
     <t>testScripts.UserModuleScripts</t>
+  </si>
+  <si>
+    <t>PASSED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,8 +122,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,6 +137,11 @@
     </fill>
     <fill>
       <patternFill patternType="gray0625">
+        <bgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
         <bgColor indexed="17"/>
       </patternFill>
     </fill>
@@ -159,13 +173,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,8 +527,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -553,8 +568,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -601,11 +616,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.44140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="32.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -638,7 +653,9 @@
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -690,11 +707,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>